<commit_message>
refs #79 Risikomanagement anpassen
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -249,9 +249,6 @@
     <t>Elaboration Iteration 3</t>
   </si>
   <si>
-    <t>Der Funktionsumfang wird reduziert, im Team wird das weitere Vorgehen besprochen,  konsultieren von externen Ressourcen (Fachexperten, Fachbücher, Fachzeitschriften etc.)</t>
-  </si>
-  <si>
     <t>Anzahl Risiken:</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>Es kommt zu Konflikten in der Projektgruppe, welche die Zusammenarbeit erschwert</t>
   </si>
   <si>
-    <t>Teambildende Massnahmen wie z.B. gemeinsame Mittagessen, sowie Ausflüge wirken dem entgegen (1x/Monat gemeinsames Abendessen)</t>
-  </si>
-  <si>
     <t>Die Situation muss bereits bei einem sich anbahnenden Konflikt besprochen werden. Vorbestimmung eines Schiedsrichters. Dieser trifft Entscheidung bei einem Problem, bei welchem nach langer Diskussion keine gemeinsame Lösung gefunden werden konnte.</t>
   </si>
   <si>
@@ -307,6 +301,15 @@
   </si>
   <si>
     <t>In der Projektvorbereitung wird ein kurzes aber intensives Literaturstudium durchgeführt und das Wissen mit Tutorials vertieft.</t>
+  </si>
+  <si>
+    <t>Der Funktionsumfang wird reduziert. Im Team wird das weitere Vorgehen besprochen,  konsultieren von externen Ressourcen (Fachexperten, Fachbücher, Fachzeitschriften etc.)</t>
+  </si>
+  <si>
+    <t>Fachwissen nicht ausreichend</t>
+  </si>
+  <si>
+    <t>Teambildende Massnahmen wie z.B. gemeinsames Mittagessen, sowie Ausflüge soll dem entgegen wirken (Einmal im Monat gemeinsames Abendessen)</t>
   </si>
 </sst>
 </file>
@@ -933,46 +936,59 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -996,39 +1012,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1369,11 +1372,11 @@
       <c r="B6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="85" t="s">
+      <c r="C6" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="90"/>
     </row>
     <row r="7" spans="1:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29"/>
@@ -1386,10 +1389,10 @@
       <c r="A8" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="34" t="s">
         <v>49</v>
       </c>
@@ -1401,10 +1404,10 @@
       <c r="A9" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="60" t="s">
         <v>62</v>
       </c>
@@ -1414,10 +1417,10 @@
       <c r="A10" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="61" t="s">
         <v>62</v>
       </c>
@@ -1427,10 +1430,10 @@
       <c r="A11" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="80"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="61" t="s">
         <v>62</v>
       </c>
@@ -1440,10 +1443,10 @@
       <c r="A12" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="80"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="61" t="s">
         <v>62</v>
       </c>
@@ -1466,10 +1469,10 @@
       <c r="A14" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="80"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="61" t="s">
         <v>62</v>
       </c>
@@ -1479,10 +1482,10 @@
       <c r="A15" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="80"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="61" t="s">
         <v>62</v>
       </c>
@@ -1492,10 +1495,10 @@
       <c r="A16" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="80"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="61" t="s">
         <v>62</v>
       </c>
@@ -1505,10 +1508,10 @@
       <c r="A17" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="80"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="61" t="s">
         <v>62</v>
       </c>
@@ -1518,10 +1521,10 @@
       <c r="A18" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="80"/>
+      <c r="C18" s="91"/>
       <c r="D18" s="61" t="s">
         <v>62</v>
       </c>
@@ -1531,10 +1534,10 @@
       <c r="A19" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="80"/>
+      <c r="C19" s="91"/>
       <c r="D19" s="61" t="s">
         <v>62</v>
       </c>
@@ -1544,10 +1547,10 @@
       <c r="A20" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="88"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="63" t="s">
         <v>62</v>
       </c>
@@ -1559,8 +1562,8 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="90"/>
-      <c r="C21" s="90"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="95"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1574,11 +1577,11 @@
       <c r="B22" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="85"/>
-      <c r="E22" s="86"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1601,10 +1604,10 @@
       <c r="A24" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="77"/>
+      <c r="C24" s="84"/>
       <c r="D24" s="34" t="s">
         <v>49</v>
       </c>
@@ -1619,8 +1622,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="82"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="60"/>
       <c r="E25" s="35"/>
       <c r="H25" s="3"/>
@@ -1631,8 +1634,8 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="58"/>
-      <c r="B26" s="78"/>
-      <c r="C26" s="79"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="61"/>
       <c r="E26" s="59"/>
       <c r="H26" s="3"/>
@@ -1643,8 +1646,8 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="79"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="61"/>
       <c r="E27" s="59"/>
       <c r="H27" s="3"/>
@@ -1655,8 +1658,8 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="58"/>
-      <c r="B28" s="78"/>
-      <c r="C28" s="79"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="61"/>
       <c r="E28" s="59"/>
       <c r="H28" s="3"/>
@@ -1667,8 +1670,8 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="84"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="62"/>
       <c r="E29" s="36"/>
     </row>
@@ -1680,11 +1683,11 @@
       <c r="B31" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="85"/>
-      <c r="E31" s="86"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="90"/>
     </row>
     <row r="32" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
@@ -1697,10 +1700,10 @@
       <c r="A33" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="77"/>
+      <c r="C33" s="84"/>
       <c r="D33" s="34" t="s">
         <v>49</v>
       </c>
@@ -1710,36 +1713,36 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="82"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="86"/>
       <c r="D34" s="60"/>
       <c r="E34" s="35"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="58"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="79"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="88"/>
       <c r="D35" s="61"/>
       <c r="E35" s="59"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="58"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="79"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="88"/>
       <c r="D36" s="61"/>
       <c r="E36" s="59"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="58"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="79"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="88"/>
       <c r="D37" s="61"/>
       <c r="E37" s="59"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="84"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="82"/>
       <c r="D38" s="62"/>
       <c r="E38" s="36"/>
     </row>
@@ -1751,11 +1754,11 @@
       <c r="B40" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="85" t="s">
+      <c r="C40" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="85"/>
-      <c r="E40" s="86"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="90"/>
     </row>
     <row r="41" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
@@ -1768,10 +1771,10 @@
       <c r="A42" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="77"/>
+      <c r="C42" s="84"/>
       <c r="D42" s="34" t="s">
         <v>49</v>
       </c>
@@ -1781,36 +1784,36 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
-      <c r="B43" s="81"/>
-      <c r="C43" s="82"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="86"/>
       <c r="D43" s="60"/>
       <c r="E43" s="35"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="58"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="79"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="88"/>
       <c r="D44" s="61"/>
       <c r="E44" s="59"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="58"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="79"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="88"/>
       <c r="D45" s="61"/>
       <c r="E45" s="59"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="58"/>
-      <c r="B46" s="78"/>
-      <c r="C46" s="79"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="88"/>
       <c r="D46" s="61"/>
       <c r="E46" s="59"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
-      <c r="B47" s="83"/>
-      <c r="C47" s="84"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="82"/>
       <c r="D47" s="62"/>
       <c r="E47" s="36"/>
     </row>
@@ -1821,11 +1824,11 @@
       <c r="B50" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="85" t="s">
+      <c r="C50" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="85"/>
-      <c r="E50" s="86"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="90"/>
     </row>
     <row r="51" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
@@ -1838,10 +1841,10 @@
       <c r="A52" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="76" t="s">
+      <c r="B52" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="77"/>
+      <c r="C52" s="84"/>
       <c r="D52" s="34" t="s">
         <v>49</v>
       </c>
@@ -1851,36 +1854,36 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
-      <c r="B53" s="81"/>
-      <c r="C53" s="82"/>
+      <c r="B53" s="85"/>
+      <c r="C53" s="86"/>
       <c r="D53" s="60"/>
       <c r="E53" s="35"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="58"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="79"/>
+      <c r="B54" s="87"/>
+      <c r="C54" s="88"/>
       <c r="D54" s="61"/>
       <c r="E54" s="59"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="58"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="79"/>
+      <c r="B55" s="87"/>
+      <c r="C55" s="88"/>
       <c r="D55" s="61"/>
       <c r="E55" s="59"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="58"/>
-      <c r="B56" s="78"/>
-      <c r="C56" s="79"/>
+      <c r="B56" s="87"/>
+      <c r="C56" s="88"/>
       <c r="D56" s="61"/>
       <c r="E56" s="59"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="32"/>
-      <c r="B57" s="83"/>
-      <c r="C57" s="84"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="82"/>
       <c r="D57" s="62"/>
       <c r="E57" s="36"/>
     </row>
@@ -1892,11 +1895,11 @@
       <c r="B59" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="85" t="s">
+      <c r="C59" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="85"/>
-      <c r="E59" s="86"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="90"/>
     </row>
     <row r="60" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A60" s="29"/>
@@ -1909,10 +1912,10 @@
       <c r="A61" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="76" t="s">
+      <c r="B61" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="77"/>
+      <c r="C61" s="84"/>
       <c r="D61" s="34" t="s">
         <v>49</v>
       </c>
@@ -1922,36 +1925,36 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
-      <c r="B62" s="81"/>
-      <c r="C62" s="82"/>
+      <c r="B62" s="85"/>
+      <c r="C62" s="86"/>
       <c r="D62" s="60"/>
       <c r="E62" s="35"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="58"/>
-      <c r="B63" s="78"/>
-      <c r="C63" s="79"/>
+      <c r="B63" s="87"/>
+      <c r="C63" s="88"/>
       <c r="D63" s="61"/>
       <c r="E63" s="59"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="58"/>
-      <c r="B64" s="78"/>
-      <c r="C64" s="79"/>
+      <c r="B64" s="87"/>
+      <c r="C64" s="88"/>
       <c r="D64" s="61"/>
       <c r="E64" s="59"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="58"/>
-      <c r="B65" s="78"/>
-      <c r="C65" s="79"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="88"/>
       <c r="D65" s="61"/>
       <c r="E65" s="59"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
-      <c r="B66" s="83"/>
-      <c r="C66" s="84"/>
+      <c r="B66" s="81"/>
+      <c r="C66" s="82"/>
       <c r="D66" s="62"/>
       <c r="E66" s="36"/>
     </row>
@@ -1962,11 +1965,11 @@
       <c r="B68" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C68" s="85" t="s">
+      <c r="C68" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D68" s="85"/>
-      <c r="E68" s="86"/>
+      <c r="D68" s="89"/>
+      <c r="E68" s="90"/>
     </row>
     <row r="69" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A69" s="29"/>
@@ -1979,10 +1982,10 @@
       <c r="A70" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B70" s="76" t="s">
+      <c r="B70" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="77"/>
+      <c r="C70" s="84"/>
       <c r="D70" s="34" t="s">
         <v>49</v>
       </c>
@@ -1992,72 +1995,49 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
-      <c r="B71" s="81"/>
-      <c r="C71" s="82"/>
+      <c r="B71" s="85"/>
+      <c r="C71" s="86"/>
       <c r="D71" s="60"/>
       <c r="E71" s="35"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="58"/>
-      <c r="B72" s="78"/>
-      <c r="C72" s="79"/>
+      <c r="B72" s="87"/>
+      <c r="C72" s="88"/>
       <c r="D72" s="61"/>
       <c r="E72" s="59"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="58"/>
-      <c r="B73" s="78"/>
-      <c r="C73" s="79"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="88"/>
       <c r="D73" s="61"/>
       <c r="E73" s="59"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="58"/>
-      <c r="B74" s="78"/>
-      <c r="C74" s="79"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="88"/>
       <c r="D74" s="61"/>
       <c r="E74" s="59"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
-      <c r="B75" s="83"/>
-      <c r="C75" s="84"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="82"/>
       <c r="D75" s="62"/>
       <c r="E75" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
@@ -2071,18 +2051,41 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2095,9 +2098,9 @@
   <dimension ref="A2:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="11" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,17 +2168,17 @@
       <c r="E6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="99"/>
+      <c r="G6" s="105"/>
       <c r="H6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="91" t="s">
+      <c r="J6" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="92"/>
+      <c r="K6" s="97"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2187,23 +2190,23 @@
       <c r="D7" s="10">
         <v>40604</v>
       </c>
-      <c r="E7" s="107">
+      <c r="E7" s="79">
         <v>1</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="106"/>
+      <c r="G7" s="103"/>
       <c r="H7" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="94"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="99"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="71">
         <f>COUNTA(A15:A51)</f>
@@ -2215,15 +2218,15 @@
       <c r="E8" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="89" t="s">
+      <c r="F8" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="106"/>
+      <c r="H8" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="97"/>
-      <c r="H8" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="99"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2231,7 +2234,7 @@
       </c>
       <c r="B9" s="71">
         <f>E26</f>
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="D9" s="75">
         <v>40609</v>
@@ -2239,44 +2242,44 @@
       <c r="E9" s="13">
         <v>1.2</v>
       </c>
-      <c r="F9" s="100" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="101"/>
+      <c r="F9" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="108"/>
       <c r="H9" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="94"/>
+        <v>76</v>
+      </c>
+      <c r="J9" s="98"/>
+      <c r="K9" s="99"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="101"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="108"/>
       <c r="H10" s="12"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="94"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="99"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="108"/>
       <c r="H11" s="12"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="96"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="101"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="102"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="76"/>
     </row>
     <row r="13" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2319,11 +2322,11 @@
       <c r="A15" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="48" t="s">
         <v>78</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>79</v>
       </c>
       <c r="D15" s="49">
         <v>10</v>
@@ -2332,13 +2335,14 @@
         <v>20</v>
       </c>
       <c r="F15" s="49">
-        <v>4</v>
+        <f>(D15/100)*E15</f>
+        <v>2</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H15" s="65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I15" s="12" t="s">
         <v>63</v>
@@ -2356,7 +2360,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="49">
         <v>15</v>
@@ -2365,14 +2369,14 @@
         <v>40</v>
       </c>
       <c r="F16" s="49">
-        <f>(D16/100)*E16</f>
+        <f t="shared" ref="F16:F24" si="0">(D16/100)*E16</f>
         <v>6</v>
       </c>
       <c r="G16" s="48" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H16" s="65" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I16" s="12" t="s">
         <v>63</v>
@@ -2386,21 +2390,21 @@
       <c r="A17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="108" t="s">
-        <v>81</v>
+      <c r="B17" s="80" t="s">
+        <v>80</v>
       </c>
       <c r="C17" s="48" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="49">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E17" s="46">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F17" s="49">
-        <f>(D17/100)*E17</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>12.5</v>
       </c>
       <c r="G17" s="48" t="s">
         <v>65</v>
@@ -2424,7 +2428,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18" s="49">
         <v>10</v>
@@ -2433,14 +2437,14 @@
         <v>150</v>
       </c>
       <c r="F18" s="49">
-        <f>(D18/100)*E18</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H18" s="65" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I18" s="74" t="s">
         <v>63</v>
@@ -2458,7 +2462,7 @@
         <v>44</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D19" s="49">
         <v>20</v>
@@ -2467,14 +2471,14 @@
         <v>30</v>
       </c>
       <c r="F19" s="49">
-        <f>(D19/100)*E19</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H19" s="65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>63</v>
@@ -2489,7 +2493,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C20" s="48" t="s">
         <v>61</v>
@@ -2501,14 +2505,14 @@
         <v>50</v>
       </c>
       <c r="F20" s="49">
-        <f>(D20/100)*E20</f>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H20" s="65" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="48" t="s">
@@ -2522,7 +2526,7 @@
       <c r="D21" s="44"/>
       <c r="E21" s="42"/>
       <c r="F21" s="49">
-        <f>(D21/100)*E21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" s="43"/>
@@ -2538,7 +2542,7 @@
       <c r="D22" s="49"/>
       <c r="E22" s="46"/>
       <c r="F22" s="49">
-        <f>(D22/100)*E22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="48"/>
@@ -2554,7 +2558,7 @@
       <c r="D23" s="49"/>
       <c r="E23" s="46"/>
       <c r="F23" s="49">
-        <f>(D23/100)*E23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="48"/>
@@ -2570,7 +2574,7 @@
       <c r="D24" s="55"/>
       <c r="E24" s="56"/>
       <c r="F24" s="44">
-        <f>(D24/100)*E24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="54"/>
@@ -2601,11 +2605,11 @@
       </c>
       <c r="E26" s="66">
         <f>SUM(E15:E24)</f>
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="F26" s="66">
         <f>SUM(F15:F24)</f>
-        <v>44.5</v>
+        <v>49</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>

</xml_diff>

<commit_message>
#refs 85 Schreibfehler korrigiert
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -276,10 +276,10 @@
     <t>HC</t>
   </si>
   <si>
-    <t>EL, TD</t>
-  </si>
-  <si>
     <t>Änderungen und Review</t>
+  </si>
+  <si>
+    <t>EL, TD,WR</t>
   </si>
 </sst>
 </file>
@@ -907,38 +907,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -949,9 +979,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -982,6 +1009,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -990,36 +1020,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1360,11 +1360,11 @@
       <c r="B6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
@@ -1377,10 +1377,10 @@
       <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="31" t="s">
         <v>30</v>
       </c>
@@ -1392,10 +1392,10 @@
       <c r="A9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="113"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="57" t="s">
         <v>40</v>
       </c>
@@ -1405,10 +1405,10 @@
       <c r="A10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="111"/>
+      <c r="C10" s="93"/>
       <c r="D10" s="58" t="s">
         <v>40</v>
       </c>
@@ -1418,10 +1418,10 @@
       <c r="A11" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="111"/>
+      <c r="C11" s="93"/>
       <c r="D11" s="58" t="s">
         <v>40</v>
       </c>
@@ -1431,10 +1431,10 @@
       <c r="A12" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="109"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="58" t="s">
         <v>40</v>
       </c>
@@ -1444,10 +1444,10 @@
       <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="109"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="58" t="s">
         <v>40</v>
       </c>
@@ -1457,10 +1457,10 @@
       <c r="A14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="111"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="58" t="s">
         <v>40</v>
       </c>
@@ -1468,15 +1468,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="58"/>
       <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
       <c r="D16" s="60"/>
       <c r="E16" s="61"/>
       <c r="H16" s="3"/>
@@ -1486,8 +1486,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="99"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1501,11 +1501,11 @@
       <c r="B18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="89"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1528,10 +1528,10 @@
       <c r="A20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1546,8 +1546,8 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="86"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="57"/>
       <c r="E21" s="32"/>
       <c r="H21" s="3"/>
@@ -1558,8 +1558,8 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="55"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="77"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="58"/>
       <c r="E22" s="56"/>
       <c r="H22" s="3"/>
@@ -1570,8 +1570,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="77"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="58"/>
       <c r="E23" s="56"/>
       <c r="H23" s="3"/>
@@ -1582,8 +1582,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="58"/>
       <c r="E24" s="56"/>
       <c r="H24" s="3"/>
@@ -1594,8 +1594,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="80"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="59"/>
       <c r="E25" s="33"/>
     </row>
@@ -1607,11 +1607,11 @@
       <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="89"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
@@ -1624,10 +1624,10 @@
       <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="84"/>
+      <c r="C29" s="83"/>
       <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
@@ -1637,36 +1637,36 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="57"/>
       <c r="E30" s="32"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="77"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="58"/>
       <c r="E31" s="56"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="77"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="87"/>
       <c r="D32" s="58"/>
       <c r="E32" s="56"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
-      <c r="B33" s="76"/>
-      <c r="C33" s="77"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
       <c r="D33" s="58"/>
       <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="80"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
       <c r="D34" s="59"/>
       <c r="E34" s="33"/>
     </row>
@@ -1678,11 +1678,11 @@
       <c r="B36" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="81" t="s">
+      <c r="C36" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="82"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="89"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="26"/>
@@ -1695,10 +1695,10 @@
       <c r="A38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="83" t="s">
+      <c r="B38" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="84"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="31" t="s">
         <v>30</v>
       </c>
@@ -1708,36 +1708,36 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="86"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="57"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
-      <c r="B40" s="76"/>
-      <c r="C40" s="77"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="87"/>
       <c r="D40" s="58"/>
       <c r="E40" s="56"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="77"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="87"/>
       <c r="D41" s="58"/>
       <c r="E41" s="56"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="77"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="87"/>
       <c r="D42" s="58"/>
       <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="80"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="81"/>
       <c r="D43" s="59"/>
       <c r="E43" s="33"/>
     </row>
@@ -1748,11 +1748,11 @@
       <c r="B46" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="81"/>
-      <c r="E46" s="82"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="89"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
@@ -1765,10 +1765,10 @@
       <c r="A48" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="83" t="s">
+      <c r="B48" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="84"/>
+      <c r="C48" s="83"/>
       <c r="D48" s="31" t="s">
         <v>30</v>
       </c>
@@ -1778,36 +1778,36 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="86"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="85"/>
       <c r="D49" s="57"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="55"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="77"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="87"/>
       <c r="D50" s="58"/>
       <c r="E50" s="56"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
-      <c r="B51" s="76"/>
-      <c r="C51" s="77"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
       <c r="D51" s="58"/>
       <c r="E51" s="56"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="77"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="87"/>
       <c r="D52" s="58"/>
       <c r="E52" s="56"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
-      <c r="B53" s="79"/>
-      <c r="C53" s="80"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="81"/>
       <c r="D53" s="59"/>
       <c r="E53" s="33"/>
     </row>
@@ -1819,11 +1819,11 @@
       <c r="B55" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="81"/>
-      <c r="E55" s="82"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="89"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
@@ -1836,10 +1836,10 @@
       <c r="A57" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="83" t="s">
+      <c r="B57" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="84"/>
+      <c r="C57" s="83"/>
       <c r="D57" s="31" t="s">
         <v>30</v>
       </c>
@@ -1849,36 +1849,36 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
-      <c r="B58" s="85"/>
-      <c r="C58" s="86"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="85"/>
       <c r="D58" s="57"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="55"/>
-      <c r="B59" s="76"/>
-      <c r="C59" s="77"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="87"/>
       <c r="D59" s="58"/>
       <c r="E59" s="56"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="55"/>
-      <c r="B60" s="76"/>
-      <c r="C60" s="77"/>
+      <c r="B60" s="86"/>
+      <c r="C60" s="87"/>
       <c r="D60" s="58"/>
       <c r="E60" s="56"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
-      <c r="B61" s="76"/>
-      <c r="C61" s="77"/>
+      <c r="B61" s="86"/>
+      <c r="C61" s="87"/>
       <c r="D61" s="58"/>
       <c r="E61" s="56"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
-      <c r="B62" s="79"/>
-      <c r="C62" s="80"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="81"/>
       <c r="D62" s="59"/>
       <c r="E62" s="33"/>
     </row>
@@ -1889,11 +1889,11 @@
       <c r="B64" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C64" s="81" t="s">
+      <c r="C64" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="82"/>
+      <c r="D64" s="88"/>
+      <c r="E64" s="89"/>
     </row>
     <row r="65" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A65" s="26"/>
@@ -1906,10 +1906,10 @@
       <c r="A66" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="83" t="s">
+      <c r="B66" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="84"/>
+      <c r="C66" s="83"/>
       <c r="D66" s="31" t="s">
         <v>30</v>
       </c>
@@ -1919,71 +1919,48 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
-      <c r="B67" s="85"/>
-      <c r="C67" s="86"/>
+      <c r="B67" s="84"/>
+      <c r="C67" s="85"/>
       <c r="D67" s="57"/>
       <c r="E67" s="32"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="55"/>
-      <c r="B68" s="76"/>
-      <c r="C68" s="77"/>
+      <c r="B68" s="86"/>
+      <c r="C68" s="87"/>
       <c r="D68" s="58"/>
       <c r="E68" s="56"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="55"/>
-      <c r="B69" s="76"/>
-      <c r="C69" s="77"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="87"/>
       <c r="D69" s="58"/>
       <c r="E69" s="56"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="55"/>
-      <c r="B70" s="76"/>
-      <c r="C70" s="77"/>
+      <c r="B70" s="86"/>
+      <c r="C70" s="87"/>
       <c r="D70" s="58"/>
       <c r="E70" s="56"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="29"/>
-      <c r="B71" s="79"/>
-      <c r="C71" s="80"/>
+      <c r="B71" s="80"/>
+      <c r="C71" s="81"/>
       <c r="D71" s="59"/>
       <c r="E71" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -2000,13 +1977,36 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2021,7 +2021,7 @@
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,17 +2089,17 @@
       <c r="E6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="100"/>
+      <c r="G6" s="109"/>
       <c r="H6" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="91" t="s">
+      <c r="J6" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="92"/>
+      <c r="K6" s="101"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2111,19 +2111,19 @@
       <c r="D7" s="10">
         <v>40604</v>
       </c>
-      <c r="E7" s="104">
+      <c r="E7" s="76">
         <v>1</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="98"/>
+      <c r="G7" s="107"/>
       <c r="H7" s="67" t="s">
         <v>77</v>
       </c>
       <c r="I7" s="74"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="94"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="103"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2136,18 +2136,18 @@
       <c r="D8" s="71">
         <v>40606</v>
       </c>
-      <c r="E8" s="105">
+      <c r="E8" s="77">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="101"/>
+      <c r="G8" s="111"/>
       <c r="H8" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="94"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2160,18 +2160,18 @@
       <c r="D9" s="71">
         <v>40609</v>
       </c>
-      <c r="E9" s="106">
+      <c r="E9" s="78">
         <v>1.2</v>
       </c>
-      <c r="F9" s="102" t="s">
+      <c r="F9" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="103"/>
+      <c r="G9" s="113"/>
       <c r="H9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="94"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="103"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2179,35 +2179,35 @@
       <c r="D10" s="71">
         <v>40609</v>
       </c>
-      <c r="E10" s="106">
+      <c r="E10" s="78">
         <v>1.3</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="112" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="113"/>
+      <c r="H10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="103"/>
-      <c r="H10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="93"/>
-      <c r="K10" s="94"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="103"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="113"/>
       <c r="H11" s="11"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="96"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="105"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="13"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="88"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="98"/>
       <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refs #214 Risiko 4&5 bereinigt
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Construction Iter2</t>
-  </si>
-  <si>
-    <t>Construction Iter3</t>
   </si>
   <si>
     <t>Transition</t>
@@ -280,6 +277,24 @@
   </si>
   <si>
     <t>EL, TD,WR</t>
+  </si>
+  <si>
+    <t>Bereinigung von Risiko 04&amp;05</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 08.03.11)</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 29.03.11)</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 12.04.11)</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 10.05.11)</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 31.05.11)</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1338,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A2:L71"/>
+  <dimension ref="A2:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A21" sqref="A21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1356,7 @@
   <sheetData>
     <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -1350,7 +1365,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="35">
-        <v>40609</v>
+        <v>40630</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
@@ -1361,7 +1376,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="D6" s="88"/>
       <c r="E6" s="89"/>
@@ -1393,11 +1408,11 @@
         <v>11</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="96"/>
       <c r="D9" s="57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="32"/>
     </row>
@@ -1406,11 +1421,11 @@
         <v>12</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="93"/>
       <c r="D10" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="56"/>
     </row>
@@ -1419,11 +1434,11 @@
         <v>13</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="93"/>
       <c r="D11" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="56"/>
     </row>
@@ -1432,11 +1447,11 @@
         <v>14</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="91"/>
       <c r="D12" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="56"/>
     </row>
@@ -1445,11 +1460,11 @@
         <v>15</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="91"/>
       <c r="D13" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="56"/>
     </row>
@@ -1458,11 +1473,11 @@
         <v>16</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="93"/>
       <c r="D14" s="58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="56"/>
     </row>
@@ -1502,7 +1517,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D18" s="88"/>
       <c r="E18" s="89"/>
@@ -1545,11 +1560,17 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="84"/>
+      <c r="A21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="84" t="s">
+        <v>73</v>
+      </c>
       <c r="C21" s="85"/>
       <c r="D21" s="57"/>
-      <c r="E21" s="32"/>
+      <c r="E21" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1557,11 +1578,17 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="86"/>
+      <c r="A22" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="87"/>
       <c r="D22" s="58"/>
-      <c r="E22" s="56"/>
+      <c r="E22" s="56" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -1608,7 +1635,7 @@
         <v>33</v>
       </c>
       <c r="C27" s="88" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D27" s="88"/>
       <c r="E27" s="89"/>
@@ -1679,7 +1706,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="88" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="D36" s="88"/>
       <c r="E36" s="89"/>
@@ -1820,7 +1847,7 @@
         <v>37</v>
       </c>
       <c r="C55" s="88" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="D55" s="88"/>
       <c r="E55" s="89"/>
@@ -1882,78 +1909,8 @@
       <c r="D62" s="59"/>
       <c r="E62" s="33"/>
     </row>
-    <row r="64" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B64" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" s="88" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="88"/>
-      <c r="E64" s="89"/>
-    </row>
-    <row r="65" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="4"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="C66" s="83"/>
-      <c r="D66" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="28"/>
-      <c r="B67" s="84"/>
-      <c r="C67" s="85"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="32"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
-      <c r="B68" s="86"/>
-      <c r="C68" s="87"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="56"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
-      <c r="B69" s="86"/>
-      <c r="C69" s="87"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="56"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="55"/>
-      <c r="B70" s="86"/>
-      <c r="C70" s="87"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="56"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
-      <c r="B71" s="80"/>
-      <c r="C71" s="81"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="33"/>
-    </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="46">
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
@@ -1986,27 +1943,20 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2018,10 +1968,10 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2012,7 @@
     </row>
     <row r="4" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="65"/>
@@ -2094,10 +2044,10 @@
       </c>
       <c r="G6" s="109"/>
       <c r="H6" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" s="100" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="101"/>
     </row>
@@ -2119,7 +2069,7 @@
       </c>
       <c r="G7" s="107"/>
       <c r="H7" s="67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="74"/>
       <c r="J7" s="102"/>
@@ -2127,7 +2077,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="68">
         <f>COUNTA(A15:A51)</f>
@@ -2140,11 +2090,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F8" s="110" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="111"/>
       <c r="H8" s="73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J8" s="102"/>
       <c r="K8" s="103"/>
@@ -2155,7 +2105,7 @@
       </c>
       <c r="B9" s="68">
         <f>F26</f>
-        <v>39.5</v>
+        <v>29.5</v>
       </c>
       <c r="D9" s="71">
         <v>40609</v>
@@ -2164,11 +2114,11 @@
         <v>1.2</v>
       </c>
       <c r="F9" s="112" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="113"/>
       <c r="H9" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="102"/>
       <c r="K9" s="103"/>
@@ -2183,11 +2133,11 @@
         <v>1.3</v>
       </c>
       <c r="F10" s="112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G10" s="113"/>
       <c r="H10" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J10" s="102"/>
       <c r="K10" s="103"/>
@@ -2195,11 +2145,19 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="112"/>
+      <c r="D11" s="71">
+        <v>40630</v>
+      </c>
+      <c r="E11" s="78">
+        <v>1.4</v>
+      </c>
+      <c r="F11" s="112" t="s">
+        <v>81</v>
+      </c>
       <c r="G11" s="113"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="J11" s="104"/>
       <c r="K11" s="105"/>
     </row>
@@ -2237,7 +2195,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>9</v>
@@ -2252,10 +2210,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="46">
         <v>2.5</v>
@@ -2268,16 +2226,16 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="I15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="J15" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" s="48"/>
     </row>
@@ -2286,10 +2244,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>53</v>
       </c>
       <c r="D16" s="46">
         <v>5</v>
@@ -2302,16 +2260,16 @@
         <v>2</v>
       </c>
       <c r="G16" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>55</v>
-      </c>
       <c r="J16" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="48"/>
     </row>
@@ -2320,10 +2278,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="46">
         <v>20</v>
@@ -2336,16 +2294,16 @@
         <v>10</v>
       </c>
       <c r="G17" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K17" s="48"/>
     </row>
@@ -2354,78 +2312,82 @@
         <v>14</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="46">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18" s="43">
         <v>50</v>
       </c>
       <c r="F18" s="46">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" s="62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I18" s="70">
         <v>143</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="48"/>
+        <v>65</v>
+      </c>
+      <c r="K18" s="48" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="46">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E19" s="43">
         <v>50</v>
       </c>
       <c r="F19" s="46">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G19" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="11">
         <v>210</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="48"/>
+        <v>65</v>
+      </c>
+      <c r="K19" s="48" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="46">
         <v>40</v>
@@ -2438,16 +2400,16 @@
         <v>16</v>
       </c>
       <c r="G20" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="H20" s="62" t="s">
+      <c r="I20" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="45" t="s">
-        <v>71</v>
-      </c>
       <c r="J20" s="45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K20" s="48"/>
     </row>
@@ -2540,7 +2502,7 @@
       </c>
       <c r="F26" s="63">
         <f>SUM(F15:F24)</f>
-        <v>39.5</v>
+        <v>29.5</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>

</xml_diff>

<commit_message>
refs #215 Review aller Risiken
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Risiko-History" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risiken!$A$14:$K$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risiken!$A$16:$K$26</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>(Anpassen bis 31.05.11)</t>
+  </si>
+  <si>
+    <t>Review nach Phase Elaboration 2</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -934,35 +937,47 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -985,15 +1000,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1035,6 +1041,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,8 +1352,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,11 +1387,11 @@
       <c r="B6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
@@ -1392,10 +1404,10 @@
       <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="83"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="31" t="s">
         <v>30</v>
       </c>
@@ -1407,10 +1419,10 @@
       <c r="A9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="96"/>
+      <c r="C9" s="100"/>
       <c r="D9" s="57" t="s">
         <v>39</v>
       </c>
@@ -1420,10 +1432,10 @@
       <c r="A10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="58" t="s">
         <v>39</v>
       </c>
@@ -1433,10 +1445,10 @@
       <c r="A11" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="93"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="58" t="s">
         <v>39</v>
       </c>
@@ -1446,10 +1458,10 @@
       <c r="A12" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="91"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="58" t="s">
         <v>39</v>
       </c>
@@ -1459,10 +1471,10 @@
       <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="91"/>
+      <c r="C13" s="95"/>
       <c r="D13" s="58" t="s">
         <v>39</v>
       </c>
@@ -1472,10 +1484,10 @@
       <c r="A14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="93"/>
+      <c r="C14" s="97"/>
       <c r="D14" s="58" t="s">
         <v>39</v>
       </c>
@@ -1483,15 +1495,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="58"/>
       <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="98"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="92"/>
       <c r="D16" s="60"/>
       <c r="E16" s="61"/>
       <c r="H16" s="3"/>
@@ -1501,8 +1513,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="99"/>
-      <c r="C17" s="99"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1516,11 +1528,11 @@
       <c r="B18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="88"/>
-      <c r="E18" s="89"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1543,10 +1555,10 @@
       <c r="A20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="83"/>
+      <c r="C20" s="84"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1563,10 +1575,10 @@
       <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="85"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="57"/>
       <c r="E21" s="32" t="s">
         <v>39</v>
@@ -1581,10 +1593,10 @@
       <c r="A22" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="87"/>
+      <c r="C22" s="88"/>
       <c r="D22" s="58"/>
       <c r="E22" s="56" t="s">
         <v>39</v>
@@ -1597,8 +1609,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="58"/>
       <c r="E23" s="56"/>
       <c r="H23" s="3"/>
@@ -1609,8 +1621,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="58"/>
       <c r="E24" s="56"/>
       <c r="H24" s="3"/>
@@ -1621,8 +1633,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="81"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="59"/>
       <c r="E25" s="33"/>
     </row>
@@ -1634,11 +1646,11 @@
       <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="89"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
@@ -1651,10 +1663,10 @@
       <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="82" t="s">
+      <c r="B29" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="83"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
@@ -1664,36 +1676,36 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="85"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="57"/>
       <c r="E30" s="32"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="87"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="58"/>
       <c r="E31" s="56"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
-      <c r="B32" s="86"/>
-      <c r="C32" s="87"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="58"/>
       <c r="E32" s="56"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
-      <c r="B33" s="86"/>
-      <c r="C33" s="87"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="58"/>
       <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
-      <c r="B34" s="80"/>
-      <c r="C34" s="81"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="59"/>
       <c r="E34" s="33"/>
     </row>
@@ -1705,11 +1717,11 @@
       <c r="B36" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="88"/>
-      <c r="E36" s="89"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="82"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="26"/>
@@ -1722,10 +1734,10 @@
       <c r="A38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="83"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="31" t="s">
         <v>30</v>
       </c>
@@ -1735,36 +1747,36 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="85"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="57"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
-      <c r="B40" s="86"/>
-      <c r="C40" s="87"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="88"/>
       <c r="D40" s="58"/>
       <c r="E40" s="56"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="87"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="88"/>
       <c r="D41" s="58"/>
       <c r="E41" s="56"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="87"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="88"/>
       <c r="D42" s="58"/>
       <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
-      <c r="B43" s="80"/>
-      <c r="C43" s="81"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="90"/>
       <c r="D43" s="59"/>
       <c r="E43" s="33"/>
     </row>
@@ -1775,11 +1787,11 @@
       <c r="B46" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="88" t="s">
+      <c r="C46" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="88"/>
-      <c r="E46" s="89"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="82"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
@@ -1792,10 +1804,10 @@
       <c r="A48" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="82" t="s">
+      <c r="B48" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="83"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="31" t="s">
         <v>30</v>
       </c>
@@ -1805,36 +1817,36 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="85"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="57"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="55"/>
-      <c r="B50" s="86"/>
-      <c r="C50" s="87"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="88"/>
       <c r="D50" s="58"/>
       <c r="E50" s="56"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
-      <c r="B51" s="86"/>
-      <c r="C51" s="87"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="88"/>
       <c r="D51" s="58"/>
       <c r="E51" s="56"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
-      <c r="B52" s="86"/>
-      <c r="C52" s="87"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="88"/>
       <c r="D52" s="58"/>
       <c r="E52" s="56"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
-      <c r="B53" s="80"/>
-      <c r="C53" s="81"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="90"/>
       <c r="D53" s="59"/>
       <c r="E53" s="33"/>
     </row>
@@ -1846,11 +1858,11 @@
       <c r="B55" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="88" t="s">
+      <c r="C55" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="D55" s="88"/>
-      <c r="E55" s="89"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="82"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
@@ -1863,10 +1875,10 @@
       <c r="A57" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="83"/>
+      <c r="C57" s="84"/>
       <c r="D57" s="31" t="s">
         <v>30</v>
       </c>
@@ -1876,48 +1888,64 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
-      <c r="B58" s="84"/>
-      <c r="C58" s="85"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="86"/>
       <c r="D58" s="57"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="55"/>
-      <c r="B59" s="86"/>
-      <c r="C59" s="87"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="88"/>
       <c r="D59" s="58"/>
       <c r="E59" s="56"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="55"/>
-      <c r="B60" s="86"/>
-      <c r="C60" s="87"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="88"/>
       <c r="D60" s="58"/>
       <c r="E60" s="56"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
-      <c r="B61" s="86"/>
-      <c r="C61" s="87"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="88"/>
       <c r="D61" s="58"/>
       <c r="E61" s="56"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
-      <c r="B62" s="80"/>
-      <c r="C62" s="81"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="90"/>
       <c r="D62" s="59"/>
       <c r="E62" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -1934,29 +1962,13 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1966,12 +1978,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A2:L31"/>
+  <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,17 +2051,17 @@
       <c r="E6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="109"/>
+      <c r="G6" s="110"/>
       <c r="H6" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="100" t="s">
+      <c r="J6" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="101"/>
+      <c r="K6" s="102"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2064,23 +2076,23 @@
       <c r="E7" s="76">
         <v>1</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="107"/>
+      <c r="G7" s="108"/>
       <c r="H7" s="67" t="s">
         <v>76</v>
       </c>
       <c r="I7" s="74"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="104"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="68">
-        <f>COUNTA(A15:A51)</f>
+        <f>COUNTA(A17:A53)</f>
         <v>6</v>
       </c>
       <c r="D8" s="71">
@@ -2089,23 +2101,23 @@
       <c r="E8" s="77">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="110" t="s">
+      <c r="F8" s="111" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="111"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="102"/>
-      <c r="K8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="104"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="68">
-        <f>F26</f>
-        <v>29.5</v>
+        <f>F28</f>
+        <v>29.1</v>
       </c>
       <c r="D9" s="71">
         <v>40609</v>
@@ -2113,15 +2125,15 @@
       <c r="E9" s="78">
         <v>1.2</v>
       </c>
-      <c r="F9" s="112" t="s">
+      <c r="F9" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="113"/>
+      <c r="G9" s="114"/>
       <c r="H9" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="102"/>
-      <c r="K9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="104"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2132,15 +2144,15 @@
       <c r="E10" s="78">
         <v>1.3</v>
       </c>
-      <c r="F10" s="112" t="s">
+      <c r="F10" s="113" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="113"/>
+      <c r="G10" s="114"/>
       <c r="H10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="102"/>
-      <c r="K10" s="103"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="104"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -2151,392 +2163,396 @@
       <c r="E11" s="78">
         <v>1.4</v>
       </c>
-      <c r="F11" s="112" t="s">
+      <c r="F11" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="113"/>
+      <c r="G11" s="114"/>
       <c r="H11" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="104"/>
-      <c r="K11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="106"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="13"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="72"/>
-    </row>
-    <row r="13" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="D12" s="71">
+        <v>40644</v>
+      </c>
+      <c r="E12" s="78">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="113" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="114"/>
+      <c r="H12" s="115" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="115"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="116"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="13"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="72"/>
+    </row>
+    <row r="15" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D16" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F16" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I16" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="102" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B17" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C17" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D17" s="46">
         <v>2.5</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E17" s="43">
         <v>60</v>
       </c>
-      <c r="F15" s="46">
-        <f>(D15/100)*E15</f>
+      <c r="F17" s="46">
+        <f>(D17/100)*E17</f>
         <v>1.5</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G17" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H17" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J17" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="48"/>
-    </row>
-    <row r="16" spans="1:12" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="K17" s="48"/>
+    </row>
+    <row r="18" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B18" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="46">
-        <v>5</v>
-      </c>
-      <c r="E16" s="43">
+      <c r="D18" s="80">
+        <v>4</v>
+      </c>
+      <c r="E18" s="43">
         <v>40</v>
       </c>
-      <c r="F16" s="46">
-        <f t="shared" ref="F16:F24" si="0">(D16/100)*E16</f>
-        <v>2</v>
-      </c>
-      <c r="G16" s="45" t="s">
+      <c r="F18" s="46">
+        <f t="shared" ref="F18:F26" si="0">(D18/100)*E18</f>
+        <v>1.6</v>
+      </c>
+      <c r="G18" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="62" t="s">
+      <c r="H18" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="45" t="s">
+      <c r="J18" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="48"/>
-    </row>
-    <row r="17" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="K18" s="48"/>
+    </row>
+    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B19" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C19" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D19" s="46">
         <v>20</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E19" s="43">
         <v>50</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F19" s="46">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G19" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H19" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="J19" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="48"/>
-    </row>
-    <row r="18" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="K19" s="48"/>
+    </row>
+    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B20" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C20" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D20" s="46">
         <v>0</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E20" s="43">
         <v>50</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F20" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G20" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="H20" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="70">
+      <c r="I20" s="70">
         <v>143</v>
       </c>
-      <c r="J18" s="45" t="s">
+      <c r="J20" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="K18" s="48" t="s">
+      <c r="K20" s="48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+    <row r="21" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B21" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C21" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="46">
+      <c r="D21" s="46">
         <v>0</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E21" s="43">
         <v>50</v>
       </c>
-      <c r="F19" s="46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="11">
-        <v>210</v>
-      </c>
-      <c r="J19" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" s="48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="75" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="46">
-        <v>40</v>
-      </c>
-      <c r="E20" s="43">
-        <v>40</v>
-      </c>
-      <c r="F20" s="46">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K20" s="48"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="39"/>
       <c r="F21" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="42"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="43"/>
+      <c r="G21" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="11">
+        <v>210</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="46">
+        <v>40</v>
+      </c>
+      <c r="E22" s="43">
+        <v>40</v>
+      </c>
       <c r="F22" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="45"/>
+        <v>16</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>42</v>
+      </c>
       <c r="K22" s="48"/>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="45"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="64"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="48"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="41">
+      <c r="A24" s="43"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="51"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="54"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="63">
-        <f>SUM(E15:E24)</f>
-        <v>290</v>
-      </c>
-      <c r="F26" s="63">
-        <f>SUM(F15:F24)</f>
-        <v>29.5</v>
-      </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="48"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="45"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="48"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="51"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="54"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="D28" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="63">
+        <f>SUM(E17:E26)</f>
+        <v>290</v>
+      </c>
+      <c r="F28" s="63">
+        <f>SUM(F17:F26)</f>
+        <v>29.1</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2575,16 +2591,42 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A14:K24">
+  <autoFilter ref="A16:K26">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <sortState ref="A15:K26">
       <sortCondition ref="A14:A26"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="8">
-    <mergeCell ref="F12:G12"/>
+  <mergeCells count="10">
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="J6:K11"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F6:G6"/>
@@ -2592,6 +2634,8 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
refs #219 Review für Abschluss Elab
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Risiko-History" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>Review nach Phase Elaboration 2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R06 </t>
+  </si>
+  <si>
+    <t>Übertragungsprobleme Mobile &lt;-&gt; Server</t>
   </si>
 </sst>
 </file>
@@ -730,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -940,35 +949,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -979,27 +1015,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1042,11 +1057,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,15 +1364,15 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -1377,7 +1389,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="35">
-        <v>40630</v>
+        <v>40646</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
@@ -1387,11 +1399,11 @@
       <c r="B6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="92"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
@@ -1404,10 +1416,10 @@
       <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="31" t="s">
         <v>30</v>
       </c>
@@ -1419,10 +1431,10 @@
       <c r="A9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="100"/>
+      <c r="C9" s="99"/>
       <c r="D9" s="57" t="s">
         <v>39</v>
       </c>
@@ -1432,10 +1444,10 @@
       <c r="A10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="97"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="58" t="s">
         <v>39</v>
       </c>
@@ -1445,10 +1457,10 @@
       <c r="A11" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="97"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="58" t="s">
         <v>39</v>
       </c>
@@ -1458,10 +1470,10 @@
       <c r="A12" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="95"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="58" t="s">
         <v>39</v>
       </c>
@@ -1471,10 +1483,10 @@
       <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="95"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="58" t="s">
         <v>39</v>
       </c>
@@ -1484,10 +1496,10 @@
       <c r="A14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="97"/>
+      <c r="C14" s="96"/>
       <c r="D14" s="58" t="s">
         <v>39</v>
       </c>
@@ -1495,15 +1507,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="97"/>
       <c r="D15" s="58"/>
       <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="60"/>
       <c r="E16" s="61"/>
       <c r="H16" s="3"/>
@@ -1513,8 +1525,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="102"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1528,11 +1540,11 @@
       <c r="B18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="92"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1555,10 +1567,10 @@
       <c r="A20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1575,10 +1587,10 @@
       <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="86"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="57"/>
       <c r="E21" s="32" t="s">
         <v>39</v>
@@ -1593,10 +1605,10 @@
       <c r="A22" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="88"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="58"/>
       <c r="E22" s="56" t="s">
         <v>39</v>
@@ -1609,8 +1621,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="58"/>
       <c r="E23" s="56"/>
       <c r="H23" s="3"/>
@@ -1621,8 +1633,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="58"/>
       <c r="E24" s="56"/>
       <c r="H24" s="3"/>
@@ -1633,8 +1645,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="84"/>
       <c r="D25" s="59"/>
       <c r="E25" s="33"/>
     </row>
@@ -1646,11 +1658,11 @@
       <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="92"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
@@ -1663,10 +1675,10 @@
       <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="84"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
@@ -1675,37 +1687,43 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
+      <c r="A30" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="117"/>
       <c r="D30" s="57"/>
-      <c r="E30" s="32"/>
+      <c r="E30" s="32" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
       <c r="D31" s="58"/>
       <c r="E31" s="56"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="88"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
       <c r="D32" s="58"/>
       <c r="E32" s="56"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="88"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="58"/>
       <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="84"/>
       <c r="D34" s="59"/>
       <c r="E34" s="33"/>
     </row>
@@ -1717,11 +1735,11 @@
       <c r="B36" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="81" t="s">
+      <c r="C36" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="82"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="92"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="26"/>
@@ -1734,10 +1752,10 @@
       <c r="A38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="83" t="s">
+      <c r="B38" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="84"/>
+      <c r="C38" s="86"/>
       <c r="D38" s="31" t="s">
         <v>30</v>
       </c>
@@ -1747,36 +1765,36 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="86"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="57"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
-      <c r="B40" s="87"/>
-      <c r="C40" s="88"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="58"/>
       <c r="E40" s="56"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
-      <c r="B41" s="87"/>
-      <c r="C41" s="88"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="90"/>
       <c r="D41" s="58"/>
       <c r="E41" s="56"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
-      <c r="B42" s="87"/>
-      <c r="C42" s="88"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="90"/>
       <c r="D42" s="58"/>
       <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="84"/>
       <c r="D43" s="59"/>
       <c r="E43" s="33"/>
     </row>
@@ -1787,11 +1805,11 @@
       <c r="B46" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="81"/>
-      <c r="E46" s="82"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="92"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
@@ -1804,10 +1822,10 @@
       <c r="A48" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="83" t="s">
+      <c r="B48" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="84"/>
+      <c r="C48" s="86"/>
       <c r="D48" s="31" t="s">
         <v>30</v>
       </c>
@@ -1817,36 +1835,36 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="86"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="88"/>
       <c r="D49" s="57"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="55"/>
-      <c r="B50" s="87"/>
-      <c r="C50" s="88"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="90"/>
       <c r="D50" s="58"/>
       <c r="E50" s="56"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
-      <c r="B51" s="87"/>
-      <c r="C51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="90"/>
       <c r="D51" s="58"/>
       <c r="E51" s="56"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
-      <c r="B52" s="87"/>
-      <c r="C52" s="88"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="90"/>
       <c r="D52" s="58"/>
       <c r="E52" s="56"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
-      <c r="B53" s="89"/>
-      <c r="C53" s="90"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="84"/>
       <c r="D53" s="59"/>
       <c r="E53" s="33"/>
     </row>
@@ -1858,11 +1876,11 @@
       <c r="B55" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="91" t="s">
         <v>86</v>
       </c>
-      <c r="D55" s="81"/>
-      <c r="E55" s="82"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="92"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
@@ -1875,10 +1893,10 @@
       <c r="A57" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="83" t="s">
+      <c r="B57" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="84"/>
+      <c r="C57" s="86"/>
       <c r="D57" s="31" t="s">
         <v>30</v>
       </c>
@@ -1888,64 +1906,48 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
-      <c r="B58" s="85"/>
-      <c r="C58" s="86"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="88"/>
       <c r="D58" s="57"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="55"/>
-      <c r="B59" s="87"/>
-      <c r="C59" s="88"/>
+      <c r="B59" s="89"/>
+      <c r="C59" s="90"/>
       <c r="D59" s="58"/>
       <c r="E59" s="56"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="55"/>
-      <c r="B60" s="87"/>
-      <c r="C60" s="88"/>
+      <c r="B60" s="89"/>
+      <c r="C60" s="90"/>
       <c r="D60" s="58"/>
       <c r="E60" s="56"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
-      <c r="B61" s="87"/>
-      <c r="C61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="90"/>
       <c r="D61" s="58"/>
       <c r="E61" s="56"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
-      <c r="B62" s="89"/>
-      <c r="C62" s="90"/>
+      <c r="B62" s="83"/>
+      <c r="C62" s="84"/>
       <c r="D62" s="59"/>
       <c r="E62" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -1962,13 +1964,29 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1980,10 +1998,10 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,17 +2069,17 @@
       <c r="E6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="109" t="s">
+      <c r="F6" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="110"/>
+      <c r="G6" s="112"/>
       <c r="H6" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="101" t="s">
+      <c r="J6" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="102"/>
+      <c r="K6" s="104"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2076,16 +2094,16 @@
       <c r="E7" s="76">
         <v>1</v>
       </c>
-      <c r="F7" s="107" t="s">
+      <c r="F7" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="108"/>
+      <c r="G7" s="110"/>
       <c r="H7" s="67" t="s">
         <v>76</v>
       </c>
       <c r="I7" s="74"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="104"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="106"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2101,15 +2119,15 @@
       <c r="E8" s="77">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="111" t="s">
+      <c r="F8" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="112"/>
+      <c r="G8" s="114"/>
       <c r="H8" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="103"/>
-      <c r="K8" s="104"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="106"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2117,7 +2135,7 @@
       </c>
       <c r="B9" s="68">
         <f>F28</f>
-        <v>29.1</v>
+        <v>13.1</v>
       </c>
       <c r="D9" s="71">
         <v>40609</v>
@@ -2125,15 +2143,15 @@
       <c r="E9" s="78">
         <v>1.2</v>
       </c>
-      <c r="F9" s="113" t="s">
+      <c r="F9" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="114"/>
+      <c r="G9" s="116"/>
       <c r="H9" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="103"/>
-      <c r="K9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="106"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2144,15 +2162,15 @@
       <c r="E10" s="78">
         <v>1.3</v>
       </c>
-      <c r="F10" s="113" t="s">
+      <c r="F10" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="114"/>
+      <c r="G10" s="116"/>
       <c r="H10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="103"/>
-      <c r="K10" s="104"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="106"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -2163,15 +2181,15 @@
       <c r="E11" s="78">
         <v>1.4</v>
       </c>
-      <c r="F11" s="113" t="s">
+      <c r="F11" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="114"/>
+      <c r="G11" s="116"/>
       <c r="H11" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="105"/>
-      <c r="K11" s="106"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="108"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -2182,32 +2200,32 @@
       <c r="E12" s="78">
         <v>1.5</v>
       </c>
-      <c r="F12" s="113" t="s">
+      <c r="F12" s="115" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="114"/>
-      <c r="H12" s="115" t="s">
+      <c r="G12" s="116"/>
+      <c r="H12" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="71"/>
       <c r="E13" s="78"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="114"/>
-      <c r="H13" s="115"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="81"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="79"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="92"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="101"/>
       <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2438,8 +2456,7 @@
         <v>40</v>
       </c>
       <c r="F22" s="46">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>68</v>
@@ -2453,7 +2470,9 @@
       <c r="J22" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="K22" s="48"/>
+      <c r="K22" s="48" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="47"/>
@@ -2544,7 +2563,7 @@
       </c>
       <c r="F28" s="63">
         <f>SUM(F17:F26)</f>
-        <v>29.1</v>
+        <v>13.1</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>

</xml_diff>

<commit_message>
refs #216 Review Risikomanagement
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="92">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -291,9 +291,6 @@
     <t>(Anpassen bis 12.04.11)</t>
   </si>
   <si>
-    <t>(Anpassen bis 10.05.11)</t>
-  </si>
-  <si>
     <t>(Anpassen bis 31.05.11)</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t>Übertragungsprobleme Mobile &lt;-&gt; Server</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 03.05.11)</t>
+  </si>
+  <si>
+    <t>Schadenspotenzial angepasst</t>
   </si>
 </sst>
 </file>
@@ -739,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -946,45 +949,54 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1006,15 +1018,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1056,9 +1059,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,8 +1364,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,11 +1399,11 @@
       <c r="B6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="91"/>
-      <c r="E6" s="92"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="83"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
@@ -1416,10 +1416,10 @@
       <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="31" t="s">
         <v>30</v>
       </c>
@@ -1431,10 +1431,10 @@
       <c r="A9" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="99"/>
+      <c r="C9" s="102"/>
       <c r="D9" s="57" t="s">
         <v>39</v>
       </c>
@@ -1444,10 +1444,10 @@
       <c r="A10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="96"/>
+      <c r="C10" s="99"/>
       <c r="D10" s="58" t="s">
         <v>39</v>
       </c>
@@ -1457,10 +1457,10 @@
       <c r="A11" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="96"/>
+      <c r="C11" s="99"/>
       <c r="D11" s="58" t="s">
         <v>39</v>
       </c>
@@ -1470,10 +1470,10 @@
       <c r="A12" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="93" t="s">
+      <c r="B12" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="94"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="58" t="s">
         <v>39</v>
       </c>
@@ -1483,10 +1483,10 @@
       <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="94"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="58" t="s">
         <v>39</v>
       </c>
@@ -1496,10 +1496,10 @@
       <c r="A14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="96"/>
+      <c r="C14" s="99"/>
       <c r="D14" s="58" t="s">
         <v>39</v>
       </c>
@@ -1507,15 +1507,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
       <c r="D15" s="58"/>
       <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
       <c r="D16" s="60"/>
       <c r="E16" s="61"/>
       <c r="H16" s="3"/>
@@ -1525,8 +1525,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="102"/>
-      <c r="C17" s="102"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1540,11 +1540,11 @@
       <c r="B18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="91"/>
-      <c r="E18" s="92"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1567,10 +1567,10 @@
       <c r="A20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1587,10 +1587,10 @@
       <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="88"/>
+      <c r="C21" s="95"/>
       <c r="D21" s="57"/>
       <c r="E21" s="32" t="s">
         <v>39</v>
@@ -1605,10 +1605,10 @@
       <c r="A22" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="90"/>
+      <c r="C22" s="89"/>
       <c r="D22" s="58"/>
       <c r="E22" s="56" t="s">
         <v>39</v>
@@ -1621,8 +1621,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="55"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="89"/>
       <c r="D23" s="58"/>
       <c r="E23" s="56"/>
       <c r="H23" s="3"/>
@@ -1633,8 +1633,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
       <c r="D24" s="58"/>
       <c r="E24" s="56"/>
       <c r="H24" s="3"/>
@@ -1645,8 +1645,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="84"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="59"/>
       <c r="E25" s="33"/>
     </row>
@@ -1658,11 +1658,11 @@
       <c r="B27" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="91" t="s">
+      <c r="C27" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="91"/>
-      <c r="E27" s="92"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="83"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
@@ -1675,10 +1675,10 @@
       <c r="A29" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="86"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
@@ -1688,12 +1688,12 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="87" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="117"/>
+      <c r="C30" s="87"/>
       <c r="D30" s="57"/>
       <c r="E30" s="32" t="s">
         <v>39</v>
@@ -1701,29 +1701,29 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
       <c r="D31" s="58"/>
       <c r="E31" s="56"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
       <c r="D32" s="58"/>
       <c r="E32" s="56"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
       <c r="D33" s="58"/>
       <c r="E33" s="56"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="84"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="91"/>
       <c r="D34" s="59"/>
       <c r="E34" s="33"/>
     </row>
@@ -1735,11 +1735,11 @@
       <c r="B36" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="91" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="91"/>
-      <c r="E36" s="92"/>
+      <c r="C36" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="26"/>
@@ -1752,10 +1752,10 @@
       <c r="A38" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="85" t="s">
+      <c r="B38" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="86"/>
+      <c r="C38" s="85"/>
       <c r="D38" s="31" t="s">
         <v>30</v>
       </c>
@@ -1765,36 +1765,36 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="88"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="95"/>
       <c r="D39" s="57"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
-      <c r="B40" s="89"/>
-      <c r="C40" s="90"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
       <c r="D40" s="58"/>
       <c r="E40" s="56"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="90"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="89"/>
       <c r="D41" s="58"/>
       <c r="E41" s="56"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="89"/>
       <c r="D42" s="58"/>
       <c r="E42" s="56"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
-      <c r="B43" s="83"/>
-      <c r="C43" s="84"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="91"/>
       <c r="D43" s="59"/>
       <c r="E43" s="33"/>
     </row>
@@ -1805,11 +1805,11 @@
       <c r="B46" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="91" t="s">
+      <c r="C46" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="83"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="26"/>
@@ -1822,10 +1822,10 @@
       <c r="A48" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="85" t="s">
+      <c r="B48" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="86"/>
+      <c r="C48" s="85"/>
       <c r="D48" s="31" t="s">
         <v>30</v>
       </c>
@@ -1835,36 +1835,36 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="87"/>
-      <c r="C49" s="88"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="95"/>
       <c r="D49" s="57"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="55"/>
-      <c r="B50" s="89"/>
-      <c r="C50" s="90"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="89"/>
       <c r="D50" s="58"/>
       <c r="E50" s="56"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
-      <c r="B51" s="89"/>
-      <c r="C51" s="90"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="89"/>
       <c r="D51" s="58"/>
       <c r="E51" s="56"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
       <c r="D52" s="58"/>
       <c r="E52" s="56"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
-      <c r="B53" s="83"/>
-      <c r="C53" s="84"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="91"/>
       <c r="D53" s="59"/>
       <c r="E53" s="33"/>
     </row>
@@ -1876,11 +1876,11 @@
       <c r="B55" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="91"/>
-      <c r="E55" s="92"/>
+      <c r="C55" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="82"/>
+      <c r="E55" s="83"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="26"/>
@@ -1893,10 +1893,10 @@
       <c r="A57" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="85" t="s">
+      <c r="B57" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="86"/>
+      <c r="C57" s="85"/>
       <c r="D57" s="31" t="s">
         <v>30</v>
       </c>
@@ -1906,48 +1906,64 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
-      <c r="B58" s="87"/>
-      <c r="C58" s="88"/>
+      <c r="B58" s="86"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="57"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="55"/>
-      <c r="B59" s="89"/>
-      <c r="C59" s="90"/>
+      <c r="B59" s="88"/>
+      <c r="C59" s="89"/>
       <c r="D59" s="58"/>
       <c r="E59" s="56"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="55"/>
-      <c r="B60" s="89"/>
-      <c r="C60" s="90"/>
+      <c r="B60" s="88"/>
+      <c r="C60" s="89"/>
       <c r="D60" s="58"/>
       <c r="E60" s="56"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
-      <c r="B61" s="89"/>
-      <c r="C61" s="90"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="89"/>
       <c r="D61" s="58"/>
       <c r="E61" s="56"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
-      <c r="B62" s="83"/>
-      <c r="C62" s="84"/>
+      <c r="B62" s="90"/>
+      <c r="C62" s="91"/>
       <c r="D62" s="59"/>
       <c r="E62" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -1964,29 +1980,13 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1999,9 +1999,9 @@
   <dimension ref="A2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="13" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="B9" s="68">
         <f>F28</f>
-        <v>13.1</v>
+        <v>7.55</v>
       </c>
       <c r="D9" s="71">
         <v>40609</v>
@@ -2201,31 +2201,39 @@
         <v>1.5</v>
       </c>
       <c r="F12" s="115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="116"/>
-      <c r="H12" s="81" t="s">
+      <c r="H12" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="115"/>
+      <c r="D13" s="71">
+        <v>40661</v>
+      </c>
+      <c r="E13" s="78">
+        <v>1.6</v>
+      </c>
+      <c r="F13" s="115" t="s">
+        <v>91</v>
+      </c>
       <c r="G13" s="116"/>
-      <c r="H13" s="81"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
+      <c r="H13" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="13"/>
       <c r="E14" s="79"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="93"/>
       <c r="H14" s="72"/>
     </row>
     <row r="15" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2279,11 +2287,11 @@
         <v>2.5</v>
       </c>
       <c r="E17" s="43">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F17" s="46">
         <f>(D17/100)*E17</f>
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="G17" s="45" t="s">
         <v>61</v>
@@ -2309,15 +2317,15 @@
       <c r="C18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="46">
         <v>4</v>
       </c>
       <c r="E18" s="43">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F18" s="46">
         <f t="shared" ref="F18:F26" si="0">(D18/100)*E18</f>
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="G18" s="45" t="s">
         <v>53</v>
@@ -2347,11 +2355,11 @@
         <v>20</v>
       </c>
       <c r="E19" s="43">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F19" s="46">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G19" s="45" t="s">
         <v>56</v>
@@ -2471,7 +2479,7 @@
         <v>42</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2559,11 +2567,11 @@
       </c>
       <c r="E28" s="63">
         <f>SUM(E17:E26)</f>
-        <v>290</v>
+        <v>220</v>
       </c>
       <c r="F28" s="63">
         <f>SUM(F17:F26)</f>
-        <v>13.1</v>
+        <v>7.55</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>

</xml_diff>

<commit_message>
refs #268 Risiken angepasst/bereinigt
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="15315" windowHeight="6090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Risiko-History" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>bereinigt</t>
-  </si>
-  <si>
-    <t>(Anpassen bis dd.mm.yyyy)</t>
   </si>
   <si>
     <t>Elaboration Iter2</t>
@@ -291,9 +288,6 @@
     <t>(Anpassen bis 12.04.11)</t>
   </si>
   <si>
-    <t>(Anpassen bis 31.05.11)</t>
-  </si>
-  <si>
     <t>Review nach Phase Elaboration 2</t>
   </si>
   <si>
@@ -306,10 +300,19 @@
     <t>Übertragungsprobleme Mobile &lt;-&gt; Server</t>
   </si>
   <si>
-    <t>(Anpassen bis 03.05.11)</t>
-  </si>
-  <si>
     <t>Schadenspotenzial angepasst</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 05.05.11)</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 19.05.11)</t>
+  </si>
+  <si>
+    <t>Schadenspotenzial nach MS5 angepasst</t>
+  </si>
+  <si>
+    <t>(Anpassen bis 03.06.11)</t>
   </si>
 </sst>
 </file>
@@ -768,9 +771,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -955,36 +955,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1006,18 +1018,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1058,6 +1058,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -1364,8 +1367,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,8 +1382,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
-        <v>38</v>
+      <c r="A2" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -1388,136 +1391,136 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="35">
-        <v>40661</v>
+      <c r="C4" s="34">
+        <v>40680</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="90" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="90"/>
-      <c r="E6" s="91"/>
+      <c r="C6" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="84"/>
+      <c r="D8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="97" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="32"/>
+      <c r="B9" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="101"/>
+      <c r="D9" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="56"/>
+      <c r="B10" s="97" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="98"/>
+      <c r="D10" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="55"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="56"/>
+      <c r="B11" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="98"/>
+      <c r="D11" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="96"/>
+      <c r="D12" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="55"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="96"/>
+      <c r="D13" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="55"/>
+    </row>
+    <row r="14" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="93"/>
-      <c r="D12" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="56"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="92" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="56"/>
-    </row>
-    <row r="14" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="56"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="56"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="55"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1525,8 +1528,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1534,17 +1537,17 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="90" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
+      <c r="B18" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1552,9 +1555,9 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
       <c r="H19" s="3"/>
@@ -1564,17 +1567,17 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="85"/>
-      <c r="D20" s="31" t="s">
+      <c r="C20" s="84"/>
+      <c r="D20" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="24" t="s">
         <v>31</v>
       </c>
       <c r="H20" s="3"/>
@@ -1584,16 +1587,16 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="32" t="s">
-        <v>39</v>
+      <c r="B21" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="94"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1602,16 +1605,16 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="89"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="56" t="s">
-        <v>39</v>
+      <c r="B22" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="88"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="55" t="s">
+        <v>38</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1620,11 +1623,11 @@
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="55"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -1632,11 +1635,11 @@
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="56"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="55"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1644,310 +1647,332 @@
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="33"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
+      <c r="B27" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="2"/>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="84" t="s">
+      <c r="B29" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="85"/>
-      <c r="D29" s="31" t="s">
+      <c r="C29" s="84"/>
+      <c r="D29" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="86" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="102"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="32" t="s">
-        <v>39</v>
+      <c r="A30" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="86"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="31" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="56"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="55"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="56"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="55"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="56"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="33"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="90"/>
-      <c r="E36" s="91"/>
+      <c r="B36" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="81"/>
+      <c r="E36" s="82"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="2"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="85"/>
-      <c r="D38" s="31" t="s">
+      <c r="C38" s="84"/>
+      <c r="D38" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="86"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="32"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="56"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="88"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="55"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="56"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="55"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="55"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="56"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="55"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="83"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="33"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="90"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="46" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="90" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" s="90"/>
-      <c r="E46" s="91"/>
+      <c r="B46" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="81"/>
+      <c r="E46" s="82"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="2"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="84" t="s">
+      <c r="B48" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="85"/>
-      <c r="D48" s="31" t="s">
+      <c r="C48" s="84"/>
+      <c r="D48" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="32"/>
+      <c r="A49" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="94"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="55"/>
-      <c r="B50" s="88"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="56"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="88"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="55"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
-      <c r="B51" s="88"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="56"/>
+      <c r="A51" s="54"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="55"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
-      <c r="B52" s="88"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="56"/>
+      <c r="A52" s="54"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="88"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="55"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="82"/>
-      <c r="C53" s="83"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="33"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="90"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C55" s="90" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="90"/>
-      <c r="E55" s="91"/>
+      <c r="B55" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="81"/>
+      <c r="E55" s="82"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="84" t="s">
+      <c r="B57" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="85"/>
-      <c r="D57" s="31" t="s">
+      <c r="C57" s="84"/>
+      <c r="D57" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
-      <c r="B58" s="86"/>
-      <c r="C58" s="87"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="32"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="94"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="55"/>
-      <c r="B59" s="88"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="56"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="55"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="55"/>
-      <c r="B60" s="88"/>
-      <c r="C60" s="89"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="56"/>
+      <c r="A60" s="54"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="88"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="55"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
-      <c r="B61" s="88"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="56"/>
+      <c r="A61" s="54"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="88"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="55"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="33"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="90"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -1964,29 +1989,13 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1998,10 +2007,10 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,15 +2050,15 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
-        <v>44</v>
+      <c r="A4" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2063,495 +2072,505 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="111" t="s">
+      <c r="F6" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="104"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="103"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="67" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="10">
         <v>40604</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="75">
         <v>1</v>
       </c>
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="110"/>
-      <c r="H7" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="106"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="105"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="68">
+        <v>44</v>
+      </c>
+      <c r="B8" s="67">
         <f>COUNTA(A17:A53)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="71">
+      <c r="D8" s="70">
         <v>40606</v>
       </c>
-      <c r="E8" s="77">
+      <c r="E8" s="76">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="113" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="114"/>
-      <c r="H8" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="105"/>
-      <c r="K8" s="106"/>
+      <c r="F8" s="112" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="113"/>
+      <c r="H8" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="104"/>
+      <c r="K8" s="105"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="67">
         <f>F28</f>
-        <v>7.55</v>
-      </c>
-      <c r="D9" s="71">
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="D9" s="70">
         <v>40609</v>
       </c>
-      <c r="E9" s="78">
+      <c r="E9" s="77">
         <v>1.2</v>
       </c>
-      <c r="F9" s="115" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="116"/>
+      <c r="F9" s="114" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="115"/>
       <c r="H9" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="105"/>
-      <c r="K9" s="106"/>
+        <v>77</v>
+      </c>
+      <c r="J9" s="104"/>
+      <c r="K9" s="105"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="D10" s="71">
+      <c r="D10" s="70">
         <v>40609</v>
       </c>
-      <c r="E10" s="78">
+      <c r="E10" s="77">
         <v>1.3</v>
       </c>
-      <c r="F10" s="115" t="s">
+      <c r="F10" s="114" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="115"/>
+      <c r="H10" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="116"/>
-      <c r="H10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="106"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="D11" s="71">
+      <c r="D11" s="70">
         <v>40630</v>
       </c>
-      <c r="E11" s="78">
+      <c r="E11" s="77">
         <v>1.4</v>
       </c>
-      <c r="F11" s="115" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="116"/>
+      <c r="F11" s="114" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="115"/>
       <c r="H11" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="107"/>
-      <c r="K11" s="108"/>
+        <v>75</v>
+      </c>
+      <c r="J11" s="106"/>
+      <c r="K11" s="107"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="D12" s="71">
+      <c r="D12" s="70">
         <v>40644</v>
       </c>
-      <c r="E12" s="78">
+      <c r="E12" s="77">
         <v>1.5</v>
       </c>
-      <c r="F12" s="115" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="116"/>
-      <c r="H12" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
+      <c r="F12" s="114" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="115"/>
+      <c r="H12" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="D13" s="71">
+      <c r="D13" s="70">
         <v>40661</v>
       </c>
-      <c r="E13" s="78">
+      <c r="E13" s="77">
         <v>1.6</v>
       </c>
-      <c r="F13" s="115" t="s">
+      <c r="F13" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="115"/>
+      <c r="H13" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="116">
+        <v>40680</v>
+      </c>
+      <c r="E14" s="78">
+        <v>1.7</v>
+      </c>
+      <c r="F14" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="116"/>
-      <c r="H13" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="13"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="72"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="71" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="18" t="s">
+      <c r="I16" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="18" t="s">
         <v>10</v>
       </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="42">
+        <v>18</v>
+      </c>
+      <c r="F17" s="45">
+        <f>(D17/100)*E17</f>
+        <v>0.45</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="47"/>
+    </row>
+    <row r="18" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="45">
+        <v>4</v>
+      </c>
+      <c r="E18" s="42">
+        <v>12</v>
+      </c>
+      <c r="F18" s="45">
+        <f t="shared" ref="F18:F26" si="0">(D18/100)*E18</f>
+        <v>0.48</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="46">
-        <v>2.5</v>
-      </c>
-      <c r="E17" s="43">
-        <v>30</v>
-      </c>
-      <c r="F17" s="46">
-        <f>(D17/100)*E17</f>
-        <v>0.75</v>
-      </c>
-      <c r="G17" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="48"/>
-    </row>
-    <row r="18" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="46">
-        <v>4</v>
-      </c>
-      <c r="E18" s="43">
-        <v>20</v>
-      </c>
-      <c r="F18" s="46">
-        <f t="shared" ref="F18:F26" si="0">(D18/100)*E18</f>
-        <v>0.8</v>
-      </c>
-      <c r="G18" s="45" t="s">
+      <c r="I18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="11" t="s">
+      <c r="J18" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="47"/>
+    </row>
+    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="J18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="48"/>
-    </row>
-    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="46">
-        <v>20</v>
-      </c>
-      <c r="E19" s="43">
-        <v>30</v>
-      </c>
-      <c r="F19" s="46">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G19" s="45" t="s">
+      <c r="C19" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="48"/>
-    </row>
-    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="46">
+      <c r="D19" s="45">
         <v>0</v>
       </c>
-      <c r="E20" s="43">
-        <v>50</v>
-      </c>
-      <c r="F20" s="46">
+      <c r="E19" s="42">
+        <v>10</v>
+      </c>
+      <c r="F19" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="70">
-        <v>143</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="48" t="s">
+      <c r="G19" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="44" t="s">
+      <c r="K19" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="46">
+      <c r="C20" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="45">
         <v>0</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E20" s="42">
         <v>50</v>
       </c>
-      <c r="F21" s="46">
+      <c r="F20" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G20" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="69">
+        <v>143</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="45">
+        <v>0</v>
+      </c>
+      <c r="E21" s="42">
         <v>50</v>
       </c>
-      <c r="H21" s="62" t="s">
-        <v>59</v>
+      <c r="F21" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>58</v>
       </c>
       <c r="I21" s="11">
         <v>210</v>
       </c>
-      <c r="J21" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" s="48" t="s">
-        <v>39</v>
+      <c r="J21" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="47" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="45" t="s">
+      <c r="B22" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="45">
+        <v>40</v>
+      </c>
+      <c r="E22" s="42">
+        <v>40</v>
+      </c>
+      <c r="F22" s="45">
+        <v>0</v>
+      </c>
+      <c r="G22" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="46">
-        <v>40</v>
-      </c>
-      <c r="E22" s="43">
-        <v>40</v>
-      </c>
-      <c r="F22" s="46">
-        <v>0</v>
-      </c>
-      <c r="G22" s="45" t="s">
+      <c r="H22" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="I22" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="K22" s="48" t="s">
-        <v>87</v>
+      <c r="J22" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="47" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="46">
+      <c r="B23" s="46"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="42"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="41"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="46">
+      <c r="A24" s="42"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="64"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="63"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="48"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="46">
+      <c r="A25" s="42"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="64"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="63"/>
       <c r="I25" s="12"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="48"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="41">
+      <c r="A26" s="48"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="51"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="54"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="53"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2562,16 +2581,16 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="62">
         <f>SUM(E17:E26)</f>
-        <v>220</v>
-      </c>
-      <c r="F28" s="63">
+        <v>180</v>
+      </c>
+      <c r="F28" s="62">
         <f>SUM(F17:F26)</f>
-        <v>7.55</v>
+        <v>0.92999999999999994</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>

</xml_diff>

<commit_message>
refs #217 Risiken bereinigt
</commit_message>
<xml_diff>
--- a/doc/01_Projektplan/risikomanagement.xlsx
+++ b/doc/01_Projektplan/risikomanagement.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risiken!$A$16:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risiken!$A$17:$K$27</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>(Anpassen bis 03.06.11)</t>
+  </si>
+  <si>
+    <t>Letzte Risiken vor Abgabe bereinigt</t>
+  </si>
+  <si>
+    <t>Konflikt im Team</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -927,9 +933,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -955,69 +958,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1060,7 +1066,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -1367,8 +1379,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="34">
-        <v>40680</v>
+        <v>40693</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
@@ -1402,11 +1414,11 @@
       <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="81"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="90"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25"/>
@@ -1434,10 +1446,10 @@
       <c r="A9" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="101"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="56" t="s">
         <v>38</v>
       </c>
@@ -1447,10 +1459,10 @@
       <c r="A10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="98"/>
+      <c r="C10" s="94"/>
       <c r="D10" s="57" t="s">
         <v>38</v>
       </c>
@@ -1460,10 +1472,10 @@
       <c r="A11" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="98"/>
+      <c r="C11" s="94"/>
       <c r="D11" s="57" t="s">
         <v>38</v>
       </c>
@@ -1473,10 +1485,10 @@
       <c r="A12" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="96"/>
+      <c r="C12" s="92"/>
       <c r="D12" s="57" t="s">
         <v>38</v>
       </c>
@@ -1486,10 +1498,10 @@
       <c r="A13" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="96"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="57" t="s">
         <v>38</v>
       </c>
@@ -1499,10 +1511,10 @@
       <c r="A14" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="98"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="57" t="s">
         <v>38</v>
       </c>
@@ -1510,15 +1522,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="57"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="57"/>
       <c r="E15" s="55"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="59"/>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="99"/>
       <c r="D16" s="59"/>
       <c r="E16" s="60"/>
       <c r="H16" s="3"/>
@@ -1528,8 +1540,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1543,11 +1555,11 @@
       <c r="B18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1593,7 +1605,7 @@
       <c r="B21" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="94"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="56"/>
       <c r="E21" s="31" t="s">
         <v>38</v>
@@ -1648,8 +1660,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="58"/>
       <c r="E25" s="32"/>
     </row>
@@ -1661,11 +1673,11 @@
       <c r="B27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="90"/>
     </row>
     <row r="28" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
@@ -1696,7 +1708,7 @@
       <c r="B30" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="86"/>
+      <c r="C30" s="101"/>
       <c r="D30" s="56"/>
       <c r="E30" s="31" t="s">
         <v>38</v>
@@ -1725,8 +1737,8 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="58"/>
       <c r="E34" s="32"/>
     </row>
@@ -1738,11 +1750,11 @@
       <c r="B36" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="81" t="s">
+      <c r="C36" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="82"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
     </row>
     <row r="37" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37" s="25"/>
@@ -1769,7 +1781,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="27"/>
       <c r="B39" s="85"/>
-      <c r="C39" s="94"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="56"/>
       <c r="E39" s="31"/>
     </row>
@@ -1796,8 +1808,8 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="82"/>
       <c r="D43" s="58"/>
       <c r="E43" s="32"/>
     </row>
@@ -1808,11 +1820,11 @@
       <c r="B46" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="81"/>
-      <c r="E46" s="82"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="90"/>
     </row>
     <row r="47" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47" s="25"/>
@@ -1843,7 +1855,7 @@
       <c r="B49" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="94"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="56"/>
       <c r="E49" s="31" t="s">
         <v>38</v>
@@ -1872,8 +1884,8 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
-      <c r="B53" s="89"/>
-      <c r="C53" s="90"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="82"/>
       <c r="D53" s="58"/>
       <c r="E53" s="32"/>
     </row>
@@ -1885,11 +1897,11 @@
       <c r="B55" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="D55" s="81"/>
-      <c r="E55" s="82"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="90"/>
     </row>
     <row r="56" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A56" s="25"/>
@@ -1914,18 +1926,30 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
-      <c r="B58" s="85"/>
-      <c r="C58" s="94"/>
+      <c r="A58" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" s="86"/>
       <c r="D58" s="56"/>
-      <c r="E58" s="31"/>
+      <c r="E58" s="31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="54"/>
-      <c r="B59" s="87"/>
+      <c r="A59" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="87" t="s">
+        <v>94</v>
+      </c>
       <c r="C59" s="88"/>
       <c r="D59" s="57"/>
-      <c r="E59" s="55"/>
+      <c r="E59" s="55" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="54"/>
@@ -1943,36 +1967,20 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
-      <c r="B62" s="89"/>
-      <c r="C62" s="90"/>
+      <c r="B62" s="81"/>
+      <c r="C62" s="82"/>
       <c r="D62" s="58"/>
       <c r="E62" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="C18:E18"/>
@@ -1989,13 +1997,29 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2005,12 +2029,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A2:L33"/>
+  <dimension ref="A2:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="14" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,14 +2052,14 @@
     <col min="11" max="11" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2049,7 +2073,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>43</v>
       </c>
@@ -2061,7 +2085,7 @@
       <c r="H4" s="65"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="D5" s="8"/>
@@ -2071,7 +2095,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="14" t="s">
         <v>17</v>
       </c>
@@ -2090,7 +2114,7 @@
       </c>
       <c r="K6" s="103"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2100,7 +2124,7 @@
       <c r="D7" s="10">
         <v>40604</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="74">
         <v>1</v>
       </c>
       <c r="F7" s="108" t="s">
@@ -2110,46 +2134,46 @@
       <c r="H7" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="73"/>
+      <c r="I7" s="72"/>
       <c r="J7" s="104"/>
       <c r="K7" s="105"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="67">
-        <f>COUNTA(A17:A53)</f>
+        <f>COUNTA(A18:A54)</f>
         <v>6</v>
       </c>
       <c r="D8" s="70">
         <v>40606</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="75">
         <v>1.1000000000000001</v>
       </c>
       <c r="F8" s="112" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="113"/>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="71" t="s">
         <v>76</v>
       </c>
       <c r="J8" s="104"/>
       <c r="K8" s="105"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="67">
-        <f>F28</f>
-        <v>0.92999999999999994</v>
+        <f>F29</f>
+        <v>0</v>
       </c>
       <c r="D9" s="70">
         <v>40609</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="76">
         <v>1.2</v>
       </c>
       <c r="F9" s="114" t="s">
@@ -2162,13 +2186,13 @@
       <c r="J9" s="104"/>
       <c r="K9" s="105"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="70">
         <v>40609</v>
       </c>
-      <c r="E10" s="77">
+      <c r="E10" s="76">
         <v>1.3</v>
       </c>
       <c r="F10" s="114" t="s">
@@ -2181,13 +2205,13 @@
       <c r="J10" s="104"/>
       <c r="K10" s="105"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="70">
         <v>40630</v>
       </c>
-      <c r="E11" s="77">
+      <c r="E11" s="76">
         <v>1.4</v>
       </c>
       <c r="F11" s="114" t="s">
@@ -2200,192 +2224,177 @@
       <c r="J11" s="106"/>
       <c r="K11" s="107"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" s="70">
         <v>40644</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="76">
         <v>1.5</v>
       </c>
       <c r="F12" s="114" t="s">
         <v>84</v>
       </c>
       <c r="G12" s="115"/>
-      <c r="H12" s="79" t="s">
+      <c r="H12" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="70">
         <v>40661</v>
       </c>
-      <c r="E13" s="77">
+      <c r="E13" s="76">
         <v>1.6</v>
       </c>
       <c r="F13" s="114" t="s">
         <v>88</v>
       </c>
       <c r="G13" s="115"/>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="116">
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="70">
         <v>40680</v>
       </c>
-      <c r="E14" s="78">
+      <c r="E14" s="76">
         <v>1.7</v>
       </c>
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="114" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="92"/>
-      <c r="H14" s="71" t="s">
+      <c r="G14" s="115"/>
+      <c r="H14" s="11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="80">
+        <v>40693</v>
+      </c>
+      <c r="E15" s="77">
+        <v>1.8</v>
+      </c>
+      <c r="F15" s="117" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="118"/>
+      <c r="H15" s="116" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B17" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F17" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H17" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I17" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K17" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="102" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B18" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C18" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="45">
+      <c r="D18" s="45">
         <v>2.5</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E18" s="42">
         <v>18</v>
       </c>
-      <c r="F17" s="45">
-        <f>(D17/100)*E17</f>
-        <v>0.45</v>
-      </c>
-      <c r="G17" s="44" t="s">
+      <c r="F18" s="45">
+        <v>0</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="61" t="s">
+      <c r="H18" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="J17" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="47"/>
-    </row>
-    <row r="18" spans="1:11" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="45">
-        <v>4</v>
-      </c>
-      <c r="E18" s="42">
-        <v>12</v>
-      </c>
-      <c r="F18" s="45">
-        <f t="shared" ref="F18:F26" si="0">(D18/100)*E18</f>
-        <v>0.48</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="J18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="47"/>
-    </row>
-    <row r="19" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="K18" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="74" t="s">
-        <v>54</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>50</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="45">
+        <v>4</v>
+      </c>
+      <c r="E19" s="42">
+        <v>12</v>
+      </c>
+      <c r="F19" s="45">
         <v>0</v>
       </c>
-      <c r="E19" s="42">
-        <v>10</v>
-      </c>
-      <c r="F19" s="45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="G19" s="44" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H19" s="61" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="J19" s="44" t="s">
         <v>39</v>
@@ -2394,51 +2403,51 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>72</v>
+        <v>13</v>
+      </c>
+      <c r="B20" s="73" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D20" s="45">
         <v>0</v>
       </c>
       <c r="E20" s="42">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F20" s="45">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F19:F27" si="0">(D20/100)*E20</f>
         <v>0</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H20" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="69">
-        <v>143</v>
+        <v>40</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="J20" s="44" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="K20" s="47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="102" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D21" s="45">
         <v>0</v>
@@ -2451,13 +2460,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="44" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H21" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="11">
-        <v>210</v>
+        <v>65</v>
+      </c>
+      <c r="I21" s="69">
+        <v>143</v>
       </c>
       <c r="J21" s="44" t="s">
         <v>64</v>
@@ -2466,73 +2475,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="102" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="74" t="s">
-        <v>73</v>
+        <v>15</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D22" s="45">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E22" s="42">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F22" s="45">
-        <v>0</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="I22" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="K22" s="47" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="41"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="G22" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="11">
+        <v>210</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="45">
+        <v>40</v>
+      </c>
+      <c r="E23" s="42">
+        <v>40</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="46"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="44"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="63"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="47"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="33"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="41"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
       <c r="B25" s="46"/>
       <c r="C25" s="44"/>
@@ -2548,70 +2577,73 @@
       <c r="J25" s="44"/>
       <c r="K25" s="47"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="40">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="53"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="50"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="53"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="62">
-        <f>SUM(E17:E26)</f>
-        <v>180</v>
-      </c>
-      <c r="F28" s="62">
-        <f>SUM(F17:F26)</f>
-        <v>0.92999999999999994</v>
-      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="D29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="62">
+        <f>SUM(E18:E27)</f>
+        <v>180</v>
+      </c>
+      <c r="F29" s="62">
+        <f>SUM(F18:F27)</f>
+        <v>0</v>
+      </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2624,7 +2656,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2637,7 +2669,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2663,16 +2695,29 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A16:K26">
+  <autoFilter ref="A17:K27">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <sortState ref="A15:K26">
       <sortCondition ref="A14:A26"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="10">
-    <mergeCell ref="F14:G14"/>
+  <mergeCells count="11">
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="J6:K11"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F6:G6"/>
@@ -2682,6 +2727,7 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>